<commit_message>
[UPDATE] insert구문 완성 및 getYoram부분 어려움 봉착
</commit_message>
<xml_diff>
--- a/2차 기획 및 테이블 구성/요라밍API명세.xlsx
+++ b/2차 기획 및 테이블 구성/요라밍API명세.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HYOTAEK\Desktop\아주대\Programing_Study\yoraming_taek\2차 기획 및 테이블 구성\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59B82F2-866C-46B0-84A2-74059FE6DDA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1235D181-F8C7-4C2D-9C02-17B1C8AC9FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="571" xr2:uid="{BBF66761-0364-4439-9B91-8813A7266E4C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="97">
   <si>
     <t>범주</t>
   </si>
@@ -410,6 +410,10 @@
   </si>
   <si>
     <t>공지사항 키워드 추가 삭제</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{success : boolean}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -812,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7E9B06-7FE6-4C64-BEF6-72E199A6C11B}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B36:B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -867,6 +871,9 @@
       <c r="F2" t="s">
         <v>31</v>
       </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B3" t="s">

</xml_diff>